<commit_message>
Improved the histogram plotting
Included some extra test such as the mann-whitney U
</commit_message>
<xml_diff>
--- a/text_files/combined_yso_parameters_v2.xlsx
+++ b/text_files/combined_yso_parameters_v2.xlsx
@@ -4424,6 +4424,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4446,6 +4447,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -4536,11 +4538,11 @@
   </sheetPr>
   <dimension ref="A1:CB35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BX1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CC25" activeCellId="0" sqref="CC25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.92"/>
@@ -4549,7 +4551,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="22" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="23.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="18.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="29" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="30.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="34.53"/>
@@ -7851,7 +7853,7 @@
         <v>0.392855759479319</v>
       </c>
       <c r="CB15" s="0" t="s">
-        <v>139</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8941,7 +8943,7 @@
         <v>0.062955826049373</v>
       </c>
       <c r="CB20" s="0" t="s">
-        <v>139</v>
+        <v>293</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>